<commit_message>
Change Some Excel(Effienciency implementation preparation
</commit_message>
<xml_diff>
--- a/DATA SMR.xlsx
+++ b/DATA SMR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matis\Desktop\Aalto S1\Advanced Energy Project\SMR-X-H2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91563113-566D-469D-9989-FDCD59ABF0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CEF522-01E2-47A6-98F8-402169571943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <sheet name="Excel Coupling Beta" sheetId="13" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SMR (Main)'!$A$1:$AE$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SMR (Main)'!$A$1:$AF$101</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="534">
   <si>
     <t>Welcome on the Main Excel for our VTT Group work for the SMR technologies comparison</t>
   </si>
@@ -1641,12 +1641,129 @@
   <si>
     <t>Ecological impact</t>
   </si>
+  <si>
+    <t>Thermal efficiency</t>
+  </si>
+  <si>
+    <t>32,5%</t>
+  </si>
+  <si>
+    <t>30,0%</t>
+  </si>
+  <si>
+    <t>30,5%</t>
+  </si>
+  <si>
+    <t>30,8%</t>
+  </si>
+  <si>
+    <t>28,9%</t>
+  </si>
+  <si>
+    <t>0,0%</t>
+  </si>
+  <si>
+    <t>32,2%</t>
+  </si>
+  <si>
+    <t>34,6%</t>
+  </si>
+  <si>
+    <t>33,3%</t>
+  </si>
+  <si>
+    <t>29,3%</t>
+  </si>
+  <si>
+    <t>30,1%</t>
+  </si>
+  <si>
+    <t>28,1%</t>
+  </si>
+  <si>
+    <t>35,0%</t>
+  </si>
+  <si>
+    <t>27,8%</t>
+  </si>
+  <si>
+    <t>31,5%</t>
+  </si>
+  <si>
+    <t>31,3%</t>
+  </si>
+  <si>
+    <t>33,9%</t>
+  </si>
+  <si>
+    <t>30,3%</t>
+  </si>
+  <si>
+    <t>40,0%</t>
+  </si>
+  <si>
+    <t>42,0%</t>
+  </si>
+  <si>
+    <t>50,0%</t>
+  </si>
+  <si>
+    <t>34,3%</t>
+  </si>
+  <si>
+    <t>43,5%</t>
+  </si>
+  <si>
+    <t>48,0%</t>
+  </si>
+  <si>
+    <t>44,9%</t>
+  </si>
+  <si>
+    <t>53,0%</t>
+  </si>
+  <si>
+    <t>44,4%</t>
+  </si>
+  <si>
+    <t>88,6%</t>
+  </si>
+  <si>
+    <t>41,3%</t>
+  </si>
+  <si>
+    <t>42,4%</t>
+  </si>
+  <si>
+    <t>40,5%</t>
+  </si>
+  <si>
+    <t>47,4%</t>
+  </si>
+  <si>
+    <t>42,9%</t>
+  </si>
+  <si>
+    <t>41,7%</t>
+  </si>
+  <si>
+    <t>35,7%</t>
+  </si>
+  <si>
+    <t>39,3%</t>
+  </si>
+  <si>
+    <t>43,8%</t>
+  </si>
+  <si>
+    <t>25,0%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1724,8 +1841,50 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1772,6 +1931,24 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -2150,7 +2327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2339,6 +2516,24 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -3366,11 +3561,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9F640B-5EF1-49D4-AF1E-498E5DBF4C83}">
-  <dimension ref="A1:AE65"/>
+  <dimension ref="A1:AF65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:AE2"/>
+      <selection pane="bottomLeft" activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3384,10 +3579,10 @@
     <col min="8" max="8" width="68" customWidth="1"/>
     <col min="9" max="10" width="15.88671875" customWidth="1"/>
     <col min="11" max="11" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="16" width="16.6640625" customWidth="1"/>
+    <col min="12" max="17" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="46" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" s="46" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
         <v>7</v>
       </c>
@@ -3433,56 +3628,59 @@
       <c r="O1" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="P1" s="76" t="s">
+        <v>495</v>
+      </c>
+      <c r="Q1" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="R1" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="S1" s="48" t="s">
         <v>493</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="T1" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="U1" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="48" t="s">
+      <c r="V1" s="48" t="s">
         <v>494</v>
       </c>
-      <c r="V1" s="48" t="s">
+      <c r="W1" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="48" t="s">
+      <c r="X1" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="48" t="s">
+      <c r="Y1" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="48" t="s">
+      <c r="Z1" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" s="48" t="s">
+      <c r="AA1" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="48" t="s">
+      <c r="AB1" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="48" t="s">
+      <c r="AC1" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="48" t="s">
+      <c r="AD1" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="48" t="s">
+      <c r="AE1" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="48" t="s">
+      <c r="AF1" s="48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="49" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" s="49" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="49" t="s">
         <v>38</v>
       </c>
@@ -3528,11 +3726,11 @@
       <c r="O2" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="49" t="s">
+      <c r="P2" s="77" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q2" s="49" t="s">
         <v>43</v>
-      </c>
-      <c r="Q2" s="49" t="s">
-        <v>44</v>
       </c>
       <c r="R2" s="49" t="s">
         <v>44</v>
@@ -3555,11 +3753,11 @@
       <c r="X2" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" s="49">
+      <c r="Y2" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z2" s="49">
         <v>10</v>
-      </c>
-      <c r="Z2" s="49" t="s">
-        <v>44</v>
       </c>
       <c r="AA2" s="49" t="s">
         <v>44</v>
@@ -3576,8 +3774,11 @@
       <c r="AE2" s="49" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AF2" s="49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>45</v>
       </c>
@@ -3617,14 +3818,14 @@
       <c r="O3" s="50">
         <v>319.5</v>
       </c>
-      <c r="P3" s="50">
+      <c r="P3" s="78" t="s">
+        <v>496</v>
+      </c>
+      <c r="Q3" s="50">
         <v>60</v>
       </c>
-      <c r="Q3" s="50">
-        <v>1</v>
-      </c>
       <c r="R3" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S3" s="50">
         <v>1</v>
@@ -3660,13 +3861,16 @@
         <v>1</v>
       </c>
       <c r="AD3" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE3" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>53</v>
       </c>
@@ -3706,12 +3910,12 @@
       <c r="O4" s="50">
         <v>326</v>
       </c>
-      <c r="P4" s="50">
+      <c r="P4" s="78" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q4" s="50">
         <v>40</v>
       </c>
-      <c r="Q4" s="50">
-        <v>1</v>
-      </c>
       <c r="R4" s="50">
         <v>1</v>
       </c>
@@ -3749,13 +3953,16 @@
         <v>1</v>
       </c>
       <c r="AD4" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="AE4" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>57</v>
       </c>
@@ -3795,14 +4002,14 @@
       <c r="O5" s="50">
         <v>321</v>
       </c>
-      <c r="P5" s="50">
+      <c r="P5" s="78" t="s">
+        <v>498</v>
+      </c>
+      <c r="Q5" s="50">
         <v>80</v>
       </c>
-      <c r="Q5" s="50">
-        <v>1</v>
-      </c>
       <c r="R5" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S5" s="50">
         <v>1</v>
@@ -3838,13 +4045,16 @@
         <v>1</v>
       </c>
       <c r="AD5" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="AE5" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>63</v>
       </c>
@@ -3884,14 +4094,14 @@
       <c r="O6" s="50">
         <v>316</v>
       </c>
-      <c r="P6" s="50">
+      <c r="P6" s="78" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q6" s="50">
         <v>60</v>
       </c>
-      <c r="Q6" s="50">
-        <v>1</v>
-      </c>
       <c r="R6" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S6" s="50">
         <v>1</v>
@@ -3927,13 +4137,16 @@
         <v>1</v>
       </c>
       <c r="AD6" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE6" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
         <v>67</v>
       </c>
@@ -3973,12 +4186,12 @@
       <c r="O7" s="50">
         <v>321</v>
       </c>
-      <c r="P7" s="50">
+      <c r="P7" s="78" t="s">
+        <v>500</v>
+      </c>
+      <c r="Q7" s="50">
         <v>60</v>
       </c>
-      <c r="Q7" s="50">
-        <v>1</v>
-      </c>
       <c r="R7" s="50">
         <v>1</v>
       </c>
@@ -4016,13 +4229,16 @@
         <v>1</v>
       </c>
       <c r="AD7" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE7" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE7" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
         <v>73</v>
       </c>
@@ -4062,12 +4278,12 @@
       <c r="O8" s="50">
         <v>120</v>
       </c>
-      <c r="P8" s="50">
+      <c r="P8" s="78" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q8" s="50">
         <v>60</v>
       </c>
-      <c r="Q8" s="50">
-        <v>1</v>
-      </c>
       <c r="R8" s="50">
         <v>1</v>
       </c>
@@ -4105,13 +4321,16 @@
         <v>1</v>
       </c>
       <c r="AD8" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE8" s="81">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="50" t="s">
         <v>77</v>
       </c>
@@ -4151,14 +4370,14 @@
       <c r="O9" s="50">
         <v>288</v>
       </c>
-      <c r="P9" s="50">
+      <c r="P9" s="78" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q9" s="50">
         <v>60</v>
       </c>
-      <c r="Q9" s="50">
-        <v>1</v>
-      </c>
       <c r="R9" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S9" s="50">
         <v>1</v>
@@ -4194,13 +4413,16 @@
         <v>1</v>
       </c>
       <c r="AD9" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE9" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="50" t="s">
         <v>82</v>
       </c>
@@ -4240,14 +4462,14 @@
       <c r="O10" s="50">
         <v>325</v>
       </c>
-      <c r="P10" s="50">
+      <c r="P10" s="78" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q10" s="50">
         <v>60</v>
       </c>
-      <c r="Q10" s="50">
-        <v>1</v>
-      </c>
       <c r="R10" s="50">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S10" s="50">
         <v>1</v>
@@ -4283,13 +4505,16 @@
         <v>1</v>
       </c>
       <c r="AD10" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE10" s="81">
+        <v>3</v>
+      </c>
+      <c r="AF10" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="50" t="s">
         <v>86</v>
       </c>
@@ -4329,14 +4554,14 @@
       <c r="O11" s="50">
         <v>285</v>
       </c>
-      <c r="P11" s="50">
+      <c r="P11" s="78" t="s">
+        <v>504</v>
+      </c>
+      <c r="Q11" s="50">
         <v>60</v>
       </c>
-      <c r="Q11" s="50">
-        <v>1</v>
-      </c>
       <c r="R11" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S11" s="50">
         <v>1</v>
@@ -4372,13 +4597,16 @@
         <v>1</v>
       </c>
       <c r="AD11" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE11" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE11" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="50" t="s">
         <v>89</v>
       </c>
@@ -4418,14 +4646,14 @@
       <c r="O12" s="50">
         <v>322</v>
       </c>
-      <c r="P12" s="50">
+      <c r="P12" s="78" t="s">
+        <v>505</v>
+      </c>
+      <c r="Q12" s="50">
         <v>60</v>
       </c>
-      <c r="Q12" s="50">
-        <v>1</v>
-      </c>
       <c r="R12" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12" s="50">
         <v>1</v>
@@ -4461,13 +4689,16 @@
         <v>1</v>
       </c>
       <c r="AD12" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE12" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE12" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF12" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="50" t="s">
         <v>93</v>
       </c>
@@ -4507,12 +4738,12 @@
       <c r="O13" s="50">
         <v>312</v>
       </c>
-      <c r="P13" s="50">
+      <c r="P13" s="78" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q13" s="50">
         <v>40</v>
       </c>
-      <c r="Q13" s="50">
-        <v>1</v>
-      </c>
       <c r="R13" s="50">
         <v>1</v>
       </c>
@@ -4550,13 +4781,16 @@
         <v>1</v>
       </c>
       <c r="AD13" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="AE13" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF13" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="50" t="s">
         <v>96</v>
       </c>
@@ -4596,14 +4830,14 @@
       <c r="O14" s="50">
         <v>324</v>
       </c>
-      <c r="P14" s="50">
+      <c r="P14" s="78" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q14" s="50">
         <v>60</v>
       </c>
-      <c r="Q14" s="50">
-        <v>1</v>
-      </c>
       <c r="R14" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S14" s="50">
         <v>1</v>
@@ -4639,13 +4873,16 @@
         <v>1</v>
       </c>
       <c r="AD14" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE14" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE14" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF14" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="50" t="s">
         <v>100</v>
       </c>
@@ -4685,14 +4922,14 @@
       <c r="O15" s="50">
         <v>345</v>
       </c>
-      <c r="P15" s="50">
+      <c r="P15" s="78" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q15" s="50">
         <v>60</v>
       </c>
-      <c r="Q15" s="50">
-        <v>1</v>
-      </c>
       <c r="R15" s="50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S15" s="50">
         <v>1</v>
@@ -4728,13 +4965,16 @@
         <v>1</v>
       </c>
       <c r="AD15" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE15" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE15" s="81">
+        <v>3</v>
+      </c>
+      <c r="AF15" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="50" t="s">
         <v>104</v>
       </c>
@@ -4774,12 +5014,12 @@
       <c r="O16" s="50">
         <v>193</v>
       </c>
-      <c r="P16" s="50">
+      <c r="P16" s="78" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q16" s="50">
         <v>60</v>
       </c>
-      <c r="Q16" s="50">
-        <v>1</v>
-      </c>
       <c r="R16" s="50">
         <v>1</v>
       </c>
@@ -4817,13 +5057,16 @@
         <v>1</v>
       </c>
       <c r="AD16" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE16" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE16" s="81">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" s="50" t="s">
         <v>111</v>
       </c>
@@ -4863,12 +5106,12 @@
       <c r="O17" s="50">
         <v>102</v>
       </c>
-      <c r="P17" s="50">
+      <c r="P17" s="78" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q17" s="50">
         <v>60</v>
       </c>
-      <c r="Q17" s="50">
-        <v>1</v>
-      </c>
       <c r="R17" s="50">
         <v>1</v>
       </c>
@@ -4906,13 +5149,16 @@
         <v>1</v>
       </c>
       <c r="AD17" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE17" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE17" s="81">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18" s="50" t="s">
         <v>115</v>
       </c>
@@ -4952,12 +5198,12 @@
       <c r="O18" s="50">
         <v>286</v>
       </c>
-      <c r="P18" s="50">
+      <c r="P18" s="78" t="s">
+        <v>509</v>
+      </c>
+      <c r="Q18" s="50">
         <v>80</v>
       </c>
-      <c r="Q18" s="50">
-        <v>1</v>
-      </c>
       <c r="R18" s="50">
         <v>1</v>
       </c>
@@ -4995,13 +5241,16 @@
         <v>1</v>
       </c>
       <c r="AD18" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE18" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="AE18" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF18" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19" s="50" t="s">
         <v>118</v>
       </c>
@@ -5041,14 +5290,14 @@
       <c r="O19" s="50">
         <v>307</v>
       </c>
-      <c r="P19" s="50">
+      <c r="P19" s="78" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q19" s="50">
         <v>60</v>
       </c>
-      <c r="Q19" s="50">
-        <v>1</v>
-      </c>
       <c r="R19" s="50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S19" s="50">
         <v>1</v>
@@ -5084,13 +5333,16 @@
         <v>1</v>
       </c>
       <c r="AD19" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE19" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE19" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF19" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20" s="50" t="s">
         <v>122</v>
       </c>
@@ -5130,14 +5382,14 @@
       <c r="O20" s="50">
         <v>310</v>
       </c>
-      <c r="P20" s="50">
+      <c r="P20" s="78" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q20" s="50">
         <v>70</v>
       </c>
-      <c r="Q20" s="50">
-        <v>1</v>
-      </c>
       <c r="R20" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S20" s="50">
         <v>1</v>
@@ -5173,13 +5425,16 @@
         <v>1</v>
       </c>
       <c r="AD20" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE20" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+        <v>8.75</v>
+      </c>
+      <c r="AE20" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF20" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A21" s="50" t="s">
         <v>128</v>
       </c>
@@ -5219,14 +5474,14 @@
       <c r="O21" s="50">
         <v>318.89999999999998</v>
       </c>
-      <c r="P21" s="50">
+      <c r="P21" s="78" t="s">
+        <v>512</v>
+      </c>
+      <c r="Q21" s="50">
         <v>60</v>
       </c>
-      <c r="Q21" s="50">
-        <v>1</v>
-      </c>
       <c r="R21" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S21" s="50">
         <v>1</v>
@@ -5262,13 +5517,16 @@
         <v>1</v>
       </c>
       <c r="AD21" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE21" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE21" s="81">
+        <v>3</v>
+      </c>
+      <c r="AF21" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A22" s="50" t="s">
         <v>131</v>
       </c>
@@ -5308,14 +5566,14 @@
       <c r="O22" s="50">
         <v>320.89999999999998</v>
       </c>
-      <c r="P22" s="50">
+      <c r="P22" s="78" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q22" s="50">
         <v>80</v>
       </c>
-      <c r="Q22" s="50">
-        <v>1</v>
-      </c>
       <c r="R22" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S22" s="50">
         <v>1</v>
@@ -5351,13 +5609,16 @@
         <v>1</v>
       </c>
       <c r="AD22" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE22" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="AE22" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF22" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A23" s="50" t="s">
         <v>135</v>
       </c>
@@ -5397,14 +5658,14 @@
       <c r="O23" s="50">
         <v>286</v>
       </c>
-      <c r="P23" s="50">
+      <c r="P23" s="78" t="s">
+        <v>509</v>
+      </c>
+      <c r="Q23" s="50">
         <v>80</v>
       </c>
-      <c r="Q23" s="50">
-        <v>1</v>
-      </c>
       <c r="R23" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S23" s="50">
         <v>1</v>
@@ -5440,13 +5701,16 @@
         <v>1</v>
       </c>
       <c r="AD23" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE23" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="AE23" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF23" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A24" s="50" t="s">
         <v>137</v>
       </c>
@@ -5486,12 +5750,12 @@
       <c r="O24" s="50">
         <v>98</v>
       </c>
-      <c r="P24" s="50">
+      <c r="P24" s="78" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q24" s="50">
         <v>60</v>
       </c>
-      <c r="Q24" s="50">
-        <v>1</v>
-      </c>
       <c r="R24" s="50">
         <v>1</v>
       </c>
@@ -5529,13 +5793,16 @@
         <v>1</v>
       </c>
       <c r="AD24" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE24" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE24" s="81">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A25" s="50" t="s">
         <v>141</v>
       </c>
@@ -5575,12 +5842,12 @@
       <c r="O25" s="50">
         <v>280</v>
       </c>
-      <c r="P25" s="50">
+      <c r="P25" s="78" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q25" s="50">
         <v>60</v>
       </c>
-      <c r="Q25" s="50">
-        <v>1</v>
-      </c>
       <c r="R25" s="50">
         <v>1</v>
       </c>
@@ -5618,13 +5885,16 @@
         <v>1</v>
       </c>
       <c r="AD25" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE25" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE25" s="81">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A26" s="50" t="s">
         <v>144</v>
       </c>
@@ -5664,14 +5934,14 @@
       <c r="O26" s="50">
         <v>313</v>
       </c>
-      <c r="P26" s="50">
+      <c r="P26" s="78" t="s">
+        <v>513</v>
+      </c>
+      <c r="Q26" s="50">
         <v>60</v>
       </c>
-      <c r="Q26" s="50">
-        <v>1</v>
-      </c>
       <c r="R26" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S26" s="50">
         <v>1</v>
@@ -5707,13 +5977,16 @@
         <v>1</v>
       </c>
       <c r="AD26" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE26" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE26" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF26" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A27" s="50" t="s">
         <v>147</v>
       </c>
@@ -5753,12 +6026,12 @@
       <c r="O27" s="50">
         <v>300</v>
       </c>
-      <c r="P27" s="50">
+      <c r="P27" s="78" t="s">
+        <v>504</v>
+      </c>
+      <c r="Q27" s="50">
         <v>60</v>
       </c>
-      <c r="Q27" s="50">
-        <v>1</v>
-      </c>
       <c r="R27" s="50">
         <v>1</v>
       </c>
@@ -5796,13 +6069,16 @@
         <v>1</v>
       </c>
       <c r="AD27" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE27" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE27" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF27" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A28" s="50" t="s">
         <v>152</v>
       </c>
@@ -5842,12 +6118,12 @@
       <c r="O28" s="50">
         <v>750</v>
       </c>
-      <c r="P28" s="50">
+      <c r="P28" s="78" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q28" s="50">
         <v>40</v>
       </c>
-      <c r="Q28" s="50">
-        <v>1</v>
-      </c>
       <c r="R28" s="50">
         <v>1</v>
       </c>
@@ -5885,13 +6161,16 @@
         <v>1</v>
       </c>
       <c r="AD28" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE28" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE28" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF28" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A29" s="50" t="s">
         <v>158</v>
       </c>
@@ -5931,14 +6210,14 @@
       <c r="O29">
         <v>750</v>
       </c>
-      <c r="P29">
+      <c r="P29" s="78" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q29">
         <v>60</v>
       </c>
-      <c r="Q29" s="50">
-        <v>1</v>
-      </c>
       <c r="R29" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S29" s="50">
         <v>1</v>
@@ -5974,13 +6253,16 @@
         <v>1</v>
       </c>
       <c r="AD29" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE29" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="AE29" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF29" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A30" s="50" t="s">
         <v>163</v>
       </c>
@@ -6020,14 +6302,14 @@
       <c r="O30">
         <v>700</v>
       </c>
-      <c r="P30">
+      <c r="P30" s="78" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q30">
         <v>20</v>
       </c>
-      <c r="Q30" s="50">
-        <v>1</v>
-      </c>
       <c r="R30" s="50">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S30" s="50">
         <v>1</v>
@@ -6063,13 +6345,16 @@
         <v>1</v>
       </c>
       <c r="AD30" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE30" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="AE30" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF30" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A31" s="50" t="s">
         <v>166</v>
       </c>
@@ -6109,14 +6394,14 @@
       <c r="O31">
         <v>900</v>
       </c>
-      <c r="P31">
+      <c r="P31" s="78" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q31">
         <v>60</v>
       </c>
-      <c r="Q31" s="50">
-        <v>1</v>
-      </c>
       <c r="R31" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S31" s="50">
         <v>1</v>
@@ -6152,13 +6437,16 @@
         <v>1</v>
       </c>
       <c r="AD31" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE31" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE31" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF31" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A32" s="50" t="s">
         <v>169</v>
       </c>
@@ -6198,12 +6486,12 @@
       <c r="O32">
         <v>850</v>
       </c>
-      <c r="P32">
+      <c r="P32" s="78" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q32">
         <v>60</v>
       </c>
-      <c r="Q32" s="50">
-        <v>1</v>
-      </c>
       <c r="R32" s="50">
         <v>1</v>
       </c>
@@ -6241,13 +6529,16 @@
         <v>1</v>
       </c>
       <c r="AD32" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE32" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+        <v>2.5</v>
+      </c>
+      <c r="AE32" s="81">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A33" s="50" t="s">
         <v>172</v>
       </c>
@@ -6287,14 +6578,14 @@
       <c r="O33">
         <v>950</v>
       </c>
-      <c r="P33">
+      <c r="P33" s="79" t="s">
+        <v>516</v>
+      </c>
+      <c r="Q33">
         <v>60</v>
       </c>
-      <c r="Q33" s="50">
-        <v>1</v>
-      </c>
       <c r="R33" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S33" s="50">
         <v>1</v>
@@ -6330,13 +6621,16 @@
         <v>1</v>
       </c>
       <c r="AD33" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE33" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE33" s="82">
+        <v>10</v>
+      </c>
+      <c r="AF33" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A34" s="50" t="s">
         <v>176</v>
       </c>
@@ -6376,14 +6670,14 @@
       <c r="O34">
         <v>800</v>
       </c>
-      <c r="P34">
+      <c r="P34" s="78" t="s">
+        <v>517</v>
+      </c>
+      <c r="Q34">
         <v>60</v>
       </c>
-      <c r="Q34" s="50">
-        <v>1</v>
-      </c>
       <c r="R34" s="50">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="S34" s="50">
         <v>1</v>
@@ -6419,13 +6713,16 @@
         <v>1</v>
       </c>
       <c r="AD34" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE34" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE34" s="81">
+        <v>3</v>
+      </c>
+      <c r="AF34" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A35" s="50" t="s">
         <v>179</v>
       </c>
@@ -6465,14 +6762,14 @@
       <c r="O35">
         <v>1200</v>
       </c>
-      <c r="P35">
+      <c r="P35" s="78" t="s">
+        <v>518</v>
+      </c>
+      <c r="Q35">
         <v>40</v>
       </c>
-      <c r="Q35" s="50">
-        <v>1</v>
-      </c>
       <c r="R35" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S35" s="50">
         <v>1</v>
@@ -6508,13 +6805,16 @@
         <v>1</v>
       </c>
       <c r="AD35" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE35" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="AE35" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF35" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A36" s="50" t="s">
         <v>183</v>
       </c>
@@ -6554,14 +6854,14 @@
       <c r="O36">
         <v>900</v>
       </c>
-      <c r="P36">
+      <c r="P36" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="Q36">
         <v>40</v>
       </c>
-      <c r="Q36" s="50">
-        <v>1</v>
-      </c>
       <c r="R36" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S36" s="50">
         <v>1</v>
@@ -6597,13 +6897,16 @@
         <v>1</v>
       </c>
       <c r="AD36" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE36" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE36" s="81">
+        <v>10</v>
+      </c>
+      <c r="AF36" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A37" s="50" t="s">
         <v>186</v>
       </c>
@@ -6643,14 +6946,14 @@
       <c r="O37">
         <v>750</v>
       </c>
-      <c r="P37">
+      <c r="P37" s="78" t="s">
+        <v>520</v>
+      </c>
+      <c r="Q37">
         <v>40</v>
       </c>
-      <c r="Q37" s="50">
-        <v>1</v>
-      </c>
       <c r="R37" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S37" s="50">
         <v>1</v>
@@ -6686,13 +6989,16 @@
         <v>1</v>
       </c>
       <c r="AD37" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE37" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="AE37" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF37" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A38" s="50" t="s">
         <v>189</v>
       </c>
@@ -6732,14 +7038,14 @@
       <c r="O38">
         <v>850</v>
       </c>
-      <c r="P38">
+      <c r="P38" s="79" t="s">
+        <v>521</v>
+      </c>
+      <c r="Q38">
         <v>60</v>
       </c>
-      <c r="Q38" s="50">
-        <v>1</v>
-      </c>
       <c r="R38" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S38" s="50">
         <v>1</v>
@@ -6775,13 +7081,16 @@
         <v>1</v>
       </c>
       <c r="AD38" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE38" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE38" s="82">
+        <v>10</v>
+      </c>
+      <c r="AF38" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A39" s="50" t="s">
         <v>194</v>
       </c>
@@ -6821,14 +7130,14 @@
       <c r="O39">
         <v>800</v>
       </c>
-      <c r="P39">
+      <c r="P39" s="78" t="s">
+        <v>522</v>
+      </c>
+      <c r="Q39">
         <v>60</v>
       </c>
-      <c r="Q39" s="50">
-        <v>1</v>
-      </c>
       <c r="R39" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S39" s="50">
         <v>1</v>
@@ -6864,13 +7173,16 @@
         <v>1</v>
       </c>
       <c r="AD39" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE39" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+        <v>3.75</v>
+      </c>
+      <c r="AE39" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF39" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A40" s="50" t="s">
         <v>197</v>
       </c>
@@ -6910,14 +7222,14 @@
       <c r="O40">
         <v>750</v>
       </c>
-      <c r="P40">
+      <c r="P40" s="80" t="s">
+        <v>523</v>
+      </c>
+      <c r="Q40">
         <v>60</v>
       </c>
-      <c r="Q40" s="50">
-        <v>1</v>
-      </c>
       <c r="R40" s="50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S40" s="50">
         <v>1</v>
@@ -6953,13 +7265,16 @@
         <v>1</v>
       </c>
       <c r="AD40" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE40" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="AE40" s="83">
+        <v>10</v>
+      </c>
+      <c r="AF40" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A41" s="50" t="s">
         <v>200</v>
       </c>
@@ -6999,14 +7314,14 @@
       <c r="O41">
         <v>750</v>
       </c>
-      <c r="P41">
+      <c r="P41" s="78" t="s">
+        <v>524</v>
+      </c>
+      <c r="Q41">
         <v>80</v>
       </c>
-      <c r="Q41" s="50">
-        <v>1</v>
-      </c>
       <c r="R41" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S41" s="50">
         <v>1</v>
@@ -7042,13 +7357,16 @@
         <v>1</v>
       </c>
       <c r="AD41" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE41" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="AE41" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF41" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A42" s="50" t="s">
         <v>204</v>
       </c>
@@ -7088,14 +7406,14 @@
       <c r="O42">
         <v>750</v>
       </c>
-      <c r="P42">
+      <c r="P42" s="78" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q42">
         <v>40</v>
       </c>
-      <c r="Q42" s="50">
-        <v>1</v>
-      </c>
       <c r="R42" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S42" s="50">
         <v>1</v>
@@ -7131,13 +7449,16 @@
         <v>1</v>
       </c>
       <c r="AD42" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE42" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE42" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF42" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A43" s="50" t="s">
         <v>208</v>
       </c>
@@ -7177,14 +7498,14 @@
       <c r="O43">
         <v>700</v>
       </c>
-      <c r="P43">
+      <c r="P43" s="78" t="s">
+        <v>525</v>
+      </c>
+      <c r="Q43">
         <v>20</v>
       </c>
-      <c r="Q43" s="50">
-        <v>1</v>
-      </c>
       <c r="R43" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S43" s="50">
         <v>1</v>
@@ -7220,13 +7541,16 @@
         <v>1</v>
       </c>
       <c r="AD43" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE43" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE43" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF43" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A44" s="50" t="s">
         <v>211</v>
       </c>
@@ -7266,14 +7590,14 @@
       <c r="O44">
         <v>850</v>
       </c>
-      <c r="P44">
+      <c r="P44" s="78" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q44">
         <v>20</v>
       </c>
-      <c r="Q44" s="50">
-        <v>1</v>
-      </c>
       <c r="R44" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S44" s="50">
         <v>1</v>
@@ -7309,13 +7633,16 @@
         <v>1</v>
       </c>
       <c r="AD44" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE44" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE44" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF44" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A45" s="51" t="s">
         <v>214</v>
       </c>
@@ -7355,14 +7682,14 @@
       <c r="O45">
         <v>650</v>
       </c>
-      <c r="P45">
+      <c r="P45" s="78" t="s">
+        <v>527</v>
+      </c>
+      <c r="Q45">
         <v>80</v>
       </c>
-      <c r="Q45" s="50">
-        <v>1</v>
-      </c>
       <c r="R45" s="50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S45" s="50">
         <v>1</v>
@@ -7398,13 +7725,16 @@
         <v>1</v>
       </c>
       <c r="AD45" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE45" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="AE45" s="81">
+        <v>10</v>
+      </c>
+      <c r="AF45" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A46" s="51" t="s">
         <v>222</v>
       </c>
@@ -7444,14 +7774,14 @@
       <c r="O46">
         <v>510</v>
       </c>
-      <c r="P46">
+      <c r="P46" s="78" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q46">
         <v>60</v>
       </c>
-      <c r="Q46" s="50">
-        <v>1</v>
-      </c>
       <c r="R46" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S46" s="50">
         <v>1</v>
@@ -7487,13 +7817,16 @@
         <v>1</v>
       </c>
       <c r="AD46" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE46" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE46" s="81">
+        <v>3</v>
+      </c>
+      <c r="AF46" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A47" s="51" t="s">
         <v>228</v>
       </c>
@@ -7533,12 +7866,12 @@
       <c r="O47">
         <v>510</v>
       </c>
-      <c r="P47">
+      <c r="P47" s="78" t="s">
+        <v>504</v>
+      </c>
+      <c r="Q47">
         <v>60</v>
       </c>
-      <c r="Q47" s="50">
-        <v>1</v>
-      </c>
       <c r="R47" s="50">
         <v>1</v>
       </c>
@@ -7576,13 +7909,16 @@
         <v>1</v>
       </c>
       <c r="AD47" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE47" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE47" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF47" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A48" s="51" t="s">
         <v>232</v>
       </c>
@@ -7622,12 +7958,12 @@
       <c r="O48">
         <v>350</v>
       </c>
-      <c r="P48">
+      <c r="P48" s="78" t="s">
+        <v>504</v>
+      </c>
+      <c r="Q48">
         <v>40</v>
       </c>
-      <c r="Q48" s="50">
-        <v>1</v>
-      </c>
       <c r="R48" s="50">
         <v>1</v>
       </c>
@@ -7665,13 +8001,16 @@
         <v>1</v>
       </c>
       <c r="AD48" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE48" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="AE48" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF48" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A49" s="51" t="s">
         <v>239</v>
       </c>
@@ -7711,14 +8050,14 @@
       <c r="O49">
         <v>535</v>
       </c>
-      <c r="P49">
+      <c r="P49" s="78" t="s">
+        <v>528</v>
+      </c>
+      <c r="Q49">
         <v>30</v>
       </c>
-      <c r="Q49" s="50">
-        <v>1</v>
-      </c>
       <c r="R49" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S49" s="50">
         <v>1</v>
@@ -7754,13 +8093,16 @@
         <v>1</v>
       </c>
       <c r="AD49" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE49" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
+        <v>3.75</v>
+      </c>
+      <c r="AE49" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF49" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A50" s="51" t="s">
         <v>245</v>
       </c>
@@ -7800,14 +8142,14 @@
       <c r="O50">
         <v>530</v>
       </c>
-      <c r="P50">
+      <c r="P50" s="78" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q50">
         <v>60</v>
       </c>
-      <c r="Q50" s="50">
-        <v>1</v>
-      </c>
       <c r="R50" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S50" s="50">
         <v>1</v>
@@ -7843,13 +8185,16 @@
         <v>1</v>
       </c>
       <c r="AD50" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE50" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE50" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF50" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A51" s="51" t="s">
         <v>248</v>
       </c>
@@ -7889,14 +8234,14 @@
       <c r="O51">
         <v>485</v>
       </c>
-      <c r="P51">
+      <c r="P51" s="78" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q51">
         <v>60</v>
       </c>
-      <c r="Q51" s="50">
-        <v>1</v>
-      </c>
       <c r="R51" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S51" s="50">
         <v>1</v>
@@ -7932,13 +8277,16 @@
         <v>1</v>
       </c>
       <c r="AD51" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE51" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE51" s="81">
+        <v>5</v>
+      </c>
+      <c r="AF51" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A52" s="51" t="s">
         <v>254</v>
       </c>
@@ -7978,12 +8326,12 @@
       <c r="O52">
         <v>550</v>
       </c>
-      <c r="P52">
+      <c r="P52" s="78" t="s">
+        <v>531</v>
+      </c>
+      <c r="Q52">
         <v>28</v>
       </c>
-      <c r="Q52" s="50">
-        <v>1</v>
-      </c>
       <c r="R52" s="50">
         <v>1</v>
       </c>
@@ -8021,13 +8369,16 @@
         <v>1</v>
       </c>
       <c r="AD52" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE52" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
+        <v>3.5</v>
+      </c>
+      <c r="AE52" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF52" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A53" s="50" t="s">
         <v>258</v>
       </c>
@@ -8067,14 +8418,14 @@
       <c r="O53">
         <v>675</v>
       </c>
-      <c r="P53" t="s">
+      <c r="P53" s="78" t="s">
+        <v>524</v>
+      </c>
+      <c r="Q53" t="s">
         <v>266</v>
       </c>
-      <c r="Q53" s="50">
-        <v>1</v>
-      </c>
       <c r="R53" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S53" s="50">
         <v>1</v>
@@ -8110,13 +8461,16 @@
         <v>1</v>
       </c>
       <c r="AD53" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE53" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE53" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF53" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A54" s="50" t="s">
         <v>267</v>
       </c>
@@ -8153,12 +8507,12 @@
       <c r="O54">
         <v>750</v>
       </c>
-      <c r="P54" t="s">
+      <c r="P54" s="79" t="s">
+        <v>516</v>
+      </c>
+      <c r="Q54" t="s">
         <v>274</v>
       </c>
-      <c r="Q54" s="50">
-        <v>1</v>
-      </c>
       <c r="R54" s="50">
         <v>1</v>
       </c>
@@ -8196,13 +8550,16 @@
         <v>1</v>
       </c>
       <c r="AD54" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE54" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="AE54" s="82">
+        <v>10</v>
+      </c>
+      <c r="AF54" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A55" s="50" t="s">
         <v>275</v>
       </c>
@@ -8242,12 +8599,12 @@
       <c r="O55">
         <v>800</v>
       </c>
-      <c r="P55">
+      <c r="P55" s="78" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q55">
         <v>60</v>
       </c>
-      <c r="Q55" s="50">
-        <v>1</v>
-      </c>
       <c r="R55" s="50">
         <v>1</v>
       </c>
@@ -8285,13 +8642,16 @@
         <v>1</v>
       </c>
       <c r="AD55" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE55" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="AE55" s="81">
+        <v>3</v>
+      </c>
+      <c r="AF55" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A56" s="50" t="s">
         <v>282</v>
       </c>
@@ -8331,12 +8691,12 @@
       <c r="O56">
         <v>700</v>
       </c>
-      <c r="P56">
+      <c r="P56" s="79" t="s">
+        <v>516</v>
+      </c>
+      <c r="Q56">
         <v>56</v>
       </c>
-      <c r="Q56" s="50">
-        <v>1</v>
-      </c>
       <c r="R56" s="50">
         <v>1</v>
       </c>
@@ -8374,13 +8734,16 @@
         <v>1</v>
       </c>
       <c r="AD56" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE56" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE56" s="82">
+        <v>10</v>
+      </c>
+      <c r="AF56" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A57" s="50" t="s">
         <v>289</v>
       </c>
@@ -8420,14 +8783,14 @@
       <c r="O57">
         <v>625</v>
       </c>
-      <c r="P57">
+      <c r="P57" s="78" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q57">
         <v>60</v>
       </c>
-      <c r="Q57" s="50">
-        <v>1</v>
-      </c>
       <c r="R57" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S57" s="50">
         <v>1</v>
@@ -8463,13 +8826,16 @@
         <v>1</v>
       </c>
       <c r="AD57" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE57" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE57" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF57" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A58" s="50" t="s">
         <v>294</v>
       </c>
@@ -8506,11 +8872,11 @@
       <c r="O58">
         <v>650</v>
       </c>
-      <c r="Q58" s="50">
-        <v>1</v>
+      <c r="P58" s="78" t="s">
+        <v>529</v>
       </c>
       <c r="R58" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S58" s="50">
         <v>1</v>
@@ -8546,13 +8912,16 @@
         <v>1</v>
       </c>
       <c r="AD58" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE58" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="AE58" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF58" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A59" s="50" t="s">
         <v>297</v>
       </c>
@@ -8592,12 +8961,12 @@
       <c r="O59">
         <v>704</v>
       </c>
-      <c r="P59">
+      <c r="P59" s="78" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q59">
         <v>80</v>
       </c>
-      <c r="Q59" s="50">
-        <v>1</v>
-      </c>
       <c r="R59" s="50">
         <v>1</v>
       </c>
@@ -8635,13 +9004,16 @@
         <v>1</v>
       </c>
       <c r="AD59" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE59" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
+        <v>0.625</v>
+      </c>
+      <c r="AE59" s="81">
+        <v>0</v>
+      </c>
+      <c r="AF59" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A60" s="50" t="s">
         <v>304</v>
       </c>
@@ -8681,12 +9053,12 @@
       <c r="O60">
         <v>704</v>
       </c>
-      <c r="P60">
+      <c r="P60" s="78" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q60">
         <v>30</v>
       </c>
-      <c r="Q60" s="50">
-        <v>1</v>
-      </c>
       <c r="R60" s="50">
         <v>1</v>
       </c>
@@ -8724,13 +9096,16 @@
         <v>1</v>
       </c>
       <c r="AD60" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE60" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="AE60" s="81">
+        <v>0</v>
+      </c>
+      <c r="AF60" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A61" s="50" t="s">
         <v>308</v>
       </c>
@@ -8770,12 +9145,12 @@
       <c r="O61">
         <v>700</v>
       </c>
-      <c r="P61">
+      <c r="P61" s="78" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q61">
         <v>60</v>
       </c>
-      <c r="Q61" s="50">
-        <v>1</v>
-      </c>
       <c r="R61" s="50">
         <v>1</v>
       </c>
@@ -8813,13 +9188,16 @@
         <v>1</v>
       </c>
       <c r="AD61" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE61" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="AE61" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF61" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A62" s="50" t="s">
         <v>315</v>
       </c>
@@ -8859,14 +9237,14 @@
       <c r="O62">
         <v>650</v>
       </c>
-      <c r="P62" t="s">
+      <c r="P62" s="78" t="s">
+        <v>532</v>
+      </c>
+      <c r="Q62" t="s">
         <v>321</v>
       </c>
-      <c r="Q62" s="50">
-        <v>1</v>
-      </c>
       <c r="R62" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S62" s="50">
         <v>1</v>
@@ -8902,13 +9280,16 @@
         <v>1</v>
       </c>
       <c r="AD62" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE62" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
+        <v>2.5</v>
+      </c>
+      <c r="AE62" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF62" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A63" s="50" t="s">
         <v>322</v>
       </c>
@@ -8948,14 +9329,14 @@
       <c r="O63">
         <v>670</v>
       </c>
-      <c r="P63" t="s">
+      <c r="P63" s="78" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q63" t="s">
         <v>327</v>
       </c>
-      <c r="Q63">
-        <v>4</v>
-      </c>
       <c r="R63" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S63" s="50">
         <v>1</v>
@@ -8991,13 +9372,16 @@
         <v>1</v>
       </c>
       <c r="AD63" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE63" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
+        <v>1.5</v>
+      </c>
+      <c r="AE63" s="81">
+        <v>9</v>
+      </c>
+      <c r="AF63" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A64" s="50" t="s">
         <v>328</v>
       </c>
@@ -9037,56 +9421,59 @@
       <c r="O64">
         <v>700</v>
       </c>
-      <c r="P64">
+      <c r="P64" s="78" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q64">
         <v>60</v>
       </c>
-      <c r="Q64">
+      <c r="R64" s="50">
+        <v>1</v>
+      </c>
+      <c r="S64" s="50">
+        <v>1</v>
+      </c>
+      <c r="T64" s="50">
+        <v>1</v>
+      </c>
+      <c r="U64" s="50">
+        <v>1</v>
+      </c>
+      <c r="V64" s="50">
+        <v>1</v>
+      </c>
+      <c r="W64" s="50">
+        <v>1</v>
+      </c>
+      <c r="X64" s="50">
+        <v>1</v>
+      </c>
+      <c r="Y64" s="50">
+        <v>1</v>
+      </c>
+      <c r="Z64" s="50">
+        <v>1</v>
+      </c>
+      <c r="AA64" s="50">
+        <v>1</v>
+      </c>
+      <c r="AB64" s="50">
+        <v>1</v>
+      </c>
+      <c r="AC64" s="50">
+        <v>1</v>
+      </c>
+      <c r="AD64" s="50">
+        <v>2.5</v>
+      </c>
+      <c r="AE64" s="81">
         <v>0</v>
       </c>
-      <c r="R64" s="50">
-        <v>1</v>
-      </c>
-      <c r="S64" s="50">
-        <v>1</v>
-      </c>
-      <c r="T64" s="50">
-        <v>1</v>
-      </c>
-      <c r="U64" s="50">
-        <v>1</v>
-      </c>
-      <c r="V64" s="50">
-        <v>1</v>
-      </c>
-      <c r="W64" s="50">
-        <v>1</v>
-      </c>
-      <c r="X64" s="50">
-        <v>1</v>
-      </c>
-      <c r="Y64" s="50">
-        <v>1</v>
-      </c>
-      <c r="Z64" s="50">
-        <v>1</v>
-      </c>
-      <c r="AA64" s="50">
-        <v>1</v>
-      </c>
-      <c r="AB64" s="50">
-        <v>1</v>
-      </c>
-      <c r="AC64" s="50">
-        <v>1</v>
-      </c>
-      <c r="AD64" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE64" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF64" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A65" s="50" t="s">
         <v>332</v>
       </c>
@@ -9126,18 +9513,18 @@
       <c r="O65">
         <v>795</v>
       </c>
-      <c r="P65">
+      <c r="P65" s="78" t="s">
+        <v>533</v>
+      </c>
+      <c r="Q65">
         <v>60</v>
       </c>
-      <c r="Q65">
-        <v>0</v>
-      </c>
-      <c r="R65">
+      <c r="R65" s="50">
+        <v>1</v>
+      </c>
+      <c r="S65">
         <v>2</v>
       </c>
-      <c r="S65" s="50">
-        <v>1</v>
-      </c>
       <c r="T65" s="50">
         <v>1</v>
       </c>
@@ -9169,14 +9556,17 @@
         <v>1</v>
       </c>
       <c r="AD65" s="50">
-        <v>1</v>
-      </c>
-      <c r="AE65" s="50">
+        <v>2.5</v>
+      </c>
+      <c r="AE65" s="81">
+        <v>1</v>
+      </c>
+      <c r="AF65" s="50">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE101" xr:uid="{9C9F640B-5EF1-49D4-AF1E-498E5DBF4C83}"/>
+  <autoFilter ref="A1:AF101" xr:uid="{9C9F640B-5EF1-49D4-AF1E-498E5DBF4C83}"/>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B65" xr:uid="{51D888AB-8CD7-42F5-B7F4-A0395698D900}"/>
   </dataValidations>
@@ -13227,25 +13617,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56528f00-8daf-4285-8b2f-184ebce7f2e9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EF98156A4E08ED42B22DA6C86624442E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11ba5f1833b47c39d11f9a0fc9ca5ad0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56528f00-8daf-4285-8b2f-184ebce7f2e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b814f87d70368c36b985d9f62a71433" ns2:_="">
     <xsd:import namespace="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
@@ -13423,25 +13794,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3D178F-0972-40B6-A2AC-EA36D3A03FFA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3162FD9B-11EE-402C-9DDF-408FEDD00CFF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56528f00-8daf-4285-8b2f-184ebce7f2e9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60EFF826-2EF8-4A64-A822-C0246D0F06D6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13457,4 +13829,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3162FD9B-11EE-402C-9DDF-408FEDD00CFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3D178F-0972-40B6-A2AC-EA36D3A03FFA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixing Excel Values+ Efficiency Calculation. Clean all the prints
</commit_message>
<xml_diff>
--- a/DATA SMR.xlsx
+++ b/DATA SMR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matis\Desktop\Aalto S1\Advanced Energy Project\SMR-X-H2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CEF522-01E2-47A6-98F8-402169571943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DC0241-06E4-4267-BA5C-5F476D11C61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="496">
   <si>
     <t>Welcome on the Main Excel for our VTT Group work for the SMR technologies comparison</t>
   </si>
@@ -1644,126 +1644,12 @@
   <si>
     <t>Thermal efficiency</t>
   </si>
-  <si>
-    <t>32,5%</t>
-  </si>
-  <si>
-    <t>30,0%</t>
-  </si>
-  <si>
-    <t>30,5%</t>
-  </si>
-  <si>
-    <t>30,8%</t>
-  </si>
-  <si>
-    <t>28,9%</t>
-  </si>
-  <si>
-    <t>0,0%</t>
-  </si>
-  <si>
-    <t>32,2%</t>
-  </si>
-  <si>
-    <t>34,6%</t>
-  </si>
-  <si>
-    <t>33,3%</t>
-  </si>
-  <si>
-    <t>29,3%</t>
-  </si>
-  <si>
-    <t>30,1%</t>
-  </si>
-  <si>
-    <t>28,1%</t>
-  </si>
-  <si>
-    <t>35,0%</t>
-  </si>
-  <si>
-    <t>27,8%</t>
-  </si>
-  <si>
-    <t>31,5%</t>
-  </si>
-  <si>
-    <t>31,3%</t>
-  </si>
-  <si>
-    <t>33,9%</t>
-  </si>
-  <si>
-    <t>30,3%</t>
-  </si>
-  <si>
-    <t>40,0%</t>
-  </si>
-  <si>
-    <t>42,0%</t>
-  </si>
-  <si>
-    <t>50,0%</t>
-  </si>
-  <si>
-    <t>34,3%</t>
-  </si>
-  <si>
-    <t>43,5%</t>
-  </si>
-  <si>
-    <t>48,0%</t>
-  </si>
-  <si>
-    <t>44,9%</t>
-  </si>
-  <si>
-    <t>53,0%</t>
-  </si>
-  <si>
-    <t>44,4%</t>
-  </si>
-  <si>
-    <t>88,6%</t>
-  </si>
-  <si>
-    <t>41,3%</t>
-  </si>
-  <si>
-    <t>42,4%</t>
-  </si>
-  <si>
-    <t>40,5%</t>
-  </si>
-  <si>
-    <t>47,4%</t>
-  </si>
-  <si>
-    <t>42,9%</t>
-  </si>
-  <si>
-    <t>41,7%</t>
-  </si>
-  <si>
-    <t>35,7%</t>
-  </si>
-  <si>
-    <t>39,3%</t>
-  </si>
-  <si>
-    <t>43,8%</t>
-  </si>
-  <si>
-    <t>25,0%</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1879,6 +1765,12 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2327,7 +2219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2492,6 +2384,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2516,24 +2426,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2990,20 +2883,20 @@
       <c r="B2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="80" t="s">
         <v>422</v>
       </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="75" t="s">
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="83" t="s">
         <v>423</v>
       </c>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
     </row>
     <row r="3" spans="1:16" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
@@ -3563,9 +3456,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9F640B-5EF1-49D4-AF1E-498E5DBF4C83}">
   <dimension ref="A1:AF65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB8" sqref="AB8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3628,7 +3521,7 @@
       <c r="O1" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="76" t="s">
+      <c r="P1" s="68" t="s">
         <v>495</v>
       </c>
       <c r="Q1" s="48" t="s">
@@ -3726,7 +3619,7 @@
       <c r="O2" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="77" t="s">
+      <c r="P2" s="69" t="s">
         <v>375</v>
       </c>
       <c r="Q2" s="49" t="s">
@@ -3818,8 +3711,8 @@
       <c r="O3" s="50">
         <v>319.5</v>
       </c>
-      <c r="P3" s="78" t="s">
-        <v>496</v>
+      <c r="P3" s="70">
+        <v>0.32500000000000001</v>
       </c>
       <c r="Q3" s="50">
         <v>60</v>
@@ -3863,7 +3756,7 @@
       <c r="AD3" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE3" s="81">
+      <c r="AE3" s="73">
         <v>1</v>
       </c>
       <c r="AF3" s="50">
@@ -3910,8 +3803,8 @@
       <c r="O4" s="50">
         <v>326</v>
       </c>
-      <c r="P4" s="78" t="s">
-        <v>497</v>
+      <c r="P4" s="70">
+        <v>0.3</v>
       </c>
       <c r="Q4" s="50">
         <v>40</v>
@@ -3955,7 +3848,7 @@
       <c r="AD4" s="50">
         <v>5</v>
       </c>
-      <c r="AE4" s="81">
+      <c r="AE4" s="73">
         <v>1</v>
       </c>
       <c r="AF4" s="50">
@@ -4002,8 +3895,8 @@
       <c r="O5" s="50">
         <v>321</v>
       </c>
-      <c r="P5" s="78" t="s">
-        <v>498</v>
+      <c r="P5" s="70">
+        <v>0.30499999999999999</v>
       </c>
       <c r="Q5" s="50">
         <v>80</v>
@@ -4047,7 +3940,7 @@
       <c r="AD5" s="50">
         <v>10</v>
       </c>
-      <c r="AE5" s="81">
+      <c r="AE5" s="73">
         <v>1</v>
       </c>
       <c r="AF5" s="50">
@@ -4094,8 +3987,8 @@
       <c r="O6" s="50">
         <v>316</v>
       </c>
-      <c r="P6" s="78" t="s">
-        <v>499</v>
+      <c r="P6" s="70">
+        <v>0.308</v>
       </c>
       <c r="Q6" s="50">
         <v>60</v>
@@ -4139,7 +4032,7 @@
       <c r="AD6" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE6" s="81">
+      <c r="AE6" s="73">
         <v>1</v>
       </c>
       <c r="AF6" s="50">
@@ -4186,8 +4079,8 @@
       <c r="O7" s="50">
         <v>321</v>
       </c>
-      <c r="P7" s="78" t="s">
-        <v>500</v>
+      <c r="P7" s="70">
+        <v>0.28899999999999998</v>
       </c>
       <c r="Q7" s="50">
         <v>60</v>
@@ -4231,7 +4124,7 @@
       <c r="AD7" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE7" s="81">
+      <c r="AE7" s="73">
         <v>1</v>
       </c>
       <c r="AF7" s="50">
@@ -4278,8 +4171,8 @@
       <c r="O8" s="50">
         <v>120</v>
       </c>
-      <c r="P8" s="78" t="s">
-        <v>501</v>
+      <c r="P8" s="70">
+        <v>0</v>
       </c>
       <c r="Q8" s="50">
         <v>60</v>
@@ -4323,7 +4216,7 @@
       <c r="AD8" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE8" s="81">
+      <c r="AE8" s="73">
         <v>0</v>
       </c>
       <c r="AF8" s="50">
@@ -4370,8 +4263,8 @@
       <c r="O9" s="50">
         <v>288</v>
       </c>
-      <c r="P9" s="78" t="s">
-        <v>502</v>
+      <c r="P9" s="70">
+        <v>0.32200000000000001</v>
       </c>
       <c r="Q9" s="50">
         <v>60</v>
@@ -4415,7 +4308,7 @@
       <c r="AD9" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE9" s="81">
+      <c r="AE9" s="73">
         <v>1</v>
       </c>
       <c r="AF9" s="50">
@@ -4462,8 +4355,8 @@
       <c r="O10" s="50">
         <v>325</v>
       </c>
-      <c r="P10" s="78" t="s">
-        <v>503</v>
+      <c r="P10" s="70">
+        <v>0.34599999999999997</v>
       </c>
       <c r="Q10" s="50">
         <v>60</v>
@@ -4507,7 +4400,7 @@
       <c r="AD10" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE10" s="81">
+      <c r="AE10" s="73">
         <v>3</v>
       </c>
       <c r="AF10" s="50">
@@ -4554,8 +4447,8 @@
       <c r="O11" s="50">
         <v>285</v>
       </c>
-      <c r="P11" s="78" t="s">
-        <v>504</v>
+      <c r="P11" s="70">
+        <v>0.33300000000000002</v>
       </c>
       <c r="Q11" s="50">
         <v>60</v>
@@ -4599,7 +4492,7 @@
       <c r="AD11" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE11" s="81">
+      <c r="AE11" s="73">
         <v>1</v>
       </c>
       <c r="AF11" s="50">
@@ -4646,8 +4539,8 @@
       <c r="O12" s="50">
         <v>322</v>
       </c>
-      <c r="P12" s="78" t="s">
-        <v>505</v>
+      <c r="P12" s="70">
+        <v>0.29299999999999998</v>
       </c>
       <c r="Q12" s="50">
         <v>60</v>
@@ -4691,7 +4584,7 @@
       <c r="AD12" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE12" s="81">
+      <c r="AE12" s="73">
         <v>1</v>
       </c>
       <c r="AF12" s="50">
@@ -4738,8 +4631,8 @@
       <c r="O13" s="50">
         <v>312</v>
       </c>
-      <c r="P13" s="78" t="s">
-        <v>506</v>
+      <c r="P13" s="70">
+        <v>0.30099999999999999</v>
       </c>
       <c r="Q13" s="50">
         <v>40</v>
@@ -4783,7 +4676,7 @@
       <c r="AD13" s="50">
         <v>5</v>
       </c>
-      <c r="AE13" s="81">
+      <c r="AE13" s="73">
         <v>1</v>
       </c>
       <c r="AF13" s="50">
@@ -4830,8 +4723,8 @@
       <c r="O14" s="50">
         <v>324</v>
       </c>
-      <c r="P14" s="78" t="s">
-        <v>507</v>
+      <c r="P14" s="70">
+        <v>0.28100000000000003</v>
       </c>
       <c r="Q14" s="50">
         <v>60</v>
@@ -4875,7 +4768,7 @@
       <c r="AD14" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE14" s="81">
+      <c r="AE14" s="73">
         <v>1</v>
       </c>
       <c r="AF14" s="50">
@@ -4922,8 +4815,8 @@
       <c r="O15" s="50">
         <v>345</v>
       </c>
-      <c r="P15" s="78" t="s">
-        <v>508</v>
+      <c r="P15" s="70">
+        <v>0.35</v>
       </c>
       <c r="Q15" s="50">
         <v>60</v>
@@ -4967,7 +4860,7 @@
       <c r="AD15" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE15" s="81">
+      <c r="AE15" s="73">
         <v>3</v>
       </c>
       <c r="AF15" s="50">
@@ -5014,8 +4907,8 @@
       <c r="O16" s="50">
         <v>193</v>
       </c>
-      <c r="P16" s="78" t="s">
-        <v>501</v>
+      <c r="P16" s="70">
+        <v>0</v>
       </c>
       <c r="Q16" s="50">
         <v>60</v>
@@ -5059,7 +4952,7 @@
       <c r="AD16" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE16" s="81">
+      <c r="AE16" s="73">
         <v>0</v>
       </c>
       <c r="AF16" s="50">
@@ -5106,8 +4999,8 @@
       <c r="O17" s="50">
         <v>102</v>
       </c>
-      <c r="P17" s="78" t="s">
-        <v>501</v>
+      <c r="P17" s="70">
+        <v>0</v>
       </c>
       <c r="Q17" s="50">
         <v>60</v>
@@ -5151,7 +5044,7 @@
       <c r="AD17" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE17" s="81">
+      <c r="AE17" s="73">
         <v>0</v>
       </c>
       <c r="AF17" s="50">
@@ -5198,8 +5091,8 @@
       <c r="O18" s="50">
         <v>286</v>
       </c>
-      <c r="P18" s="78" t="s">
-        <v>509</v>
+      <c r="P18" s="70">
+        <v>0.27800000000000002</v>
       </c>
       <c r="Q18" s="50">
         <v>80</v>
@@ -5243,7 +5136,7 @@
       <c r="AD18" s="50">
         <v>10</v>
       </c>
-      <c r="AE18" s="81">
+      <c r="AE18" s="73">
         <v>1</v>
       </c>
       <c r="AF18" s="50">
@@ -5290,13 +5183,13 @@
       <c r="O19" s="50">
         <v>307</v>
       </c>
-      <c r="P19" s="78" t="s">
-        <v>510</v>
+      <c r="P19" s="70">
+        <v>0</v>
       </c>
       <c r="Q19" s="50">
         <v>60</v>
       </c>
-      <c r="R19" s="50">
+      <c r="R19" s="84">
         <v>4</v>
       </c>
       <c r="S19" s="50">
@@ -5335,7 +5228,7 @@
       <c r="AD19" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE19" s="81">
+      <c r="AE19" s="73">
         <v>1</v>
       </c>
       <c r="AF19" s="50">
@@ -5382,8 +5275,8 @@
       <c r="O20" s="50">
         <v>310</v>
       </c>
-      <c r="P20" s="78" t="s">
-        <v>511</v>
+      <c r="P20" s="70">
+        <v>0.313</v>
       </c>
       <c r="Q20" s="50">
         <v>70</v>
@@ -5427,7 +5320,7 @@
       <c r="AD20" s="50">
         <v>8.75</v>
       </c>
-      <c r="AE20" s="81">
+      <c r="AE20" s="73">
         <v>1</v>
       </c>
       <c r="AF20" s="50">
@@ -5474,8 +5367,8 @@
       <c r="O21" s="50">
         <v>318.89999999999998</v>
       </c>
-      <c r="P21" s="78" t="s">
-        <v>512</v>
+      <c r="P21" s="70">
+        <v>0.33900000000000002</v>
       </c>
       <c r="Q21" s="50">
         <v>60</v>
@@ -5519,7 +5412,7 @@
       <c r="AD21" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE21" s="81">
+      <c r="AE21" s="73">
         <v>3</v>
       </c>
       <c r="AF21" s="50">
@@ -5566,8 +5459,8 @@
       <c r="O22" s="50">
         <v>320.89999999999998</v>
       </c>
-      <c r="P22" s="78" t="s">
-        <v>510</v>
+      <c r="P22" s="70">
+        <v>0.315</v>
       </c>
       <c r="Q22" s="50">
         <v>80</v>
@@ -5611,7 +5504,7 @@
       <c r="AD22" s="50">
         <v>10</v>
       </c>
-      <c r="AE22" s="81">
+      <c r="AE22" s="73">
         <v>1</v>
       </c>
       <c r="AF22" s="50">
@@ -5658,8 +5551,8 @@
       <c r="O23" s="50">
         <v>286</v>
       </c>
-      <c r="P23" s="78" t="s">
-        <v>509</v>
+      <c r="P23" s="70">
+        <v>0.27800000000000002</v>
       </c>
       <c r="Q23" s="50">
         <v>80</v>
@@ -5703,7 +5596,7 @@
       <c r="AD23" s="50">
         <v>10</v>
       </c>
-      <c r="AE23" s="81">
+      <c r="AE23" s="73">
         <v>1</v>
       </c>
       <c r="AF23" s="50">
@@ -5750,8 +5643,8 @@
       <c r="O24" s="50">
         <v>98</v>
       </c>
-      <c r="P24" s="78" t="s">
-        <v>501</v>
+      <c r="P24" s="70">
+        <v>0</v>
       </c>
       <c r="Q24" s="50">
         <v>60</v>
@@ -5795,7 +5688,7 @@
       <c r="AD24" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE24" s="81">
+      <c r="AE24" s="73">
         <v>0</v>
       </c>
       <c r="AF24" s="50">
@@ -5842,8 +5735,8 @@
       <c r="O25" s="50">
         <v>280</v>
       </c>
-      <c r="P25" s="78" t="s">
-        <v>501</v>
+      <c r="P25" s="70">
+        <v>0</v>
       </c>
       <c r="Q25" s="50">
         <v>60</v>
@@ -5887,7 +5780,7 @@
       <c r="AD25" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE25" s="81">
+      <c r="AE25" s="73">
         <v>0</v>
       </c>
       <c r="AF25" s="50">
@@ -5934,8 +5827,8 @@
       <c r="O26" s="50">
         <v>313</v>
       </c>
-      <c r="P26" s="78" t="s">
-        <v>513</v>
+      <c r="P26" s="70">
+        <v>0.30299999999999999</v>
       </c>
       <c r="Q26" s="50">
         <v>60</v>
@@ -5979,7 +5872,7 @@
       <c r="AD26" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE26" s="81">
+      <c r="AE26" s="73">
         <v>1</v>
       </c>
       <c r="AF26" s="50">
@@ -6026,8 +5919,8 @@
       <c r="O27" s="50">
         <v>300</v>
       </c>
-      <c r="P27" s="78" t="s">
-        <v>504</v>
+      <c r="P27" s="70">
+        <v>0.33300000000000002</v>
       </c>
       <c r="Q27" s="50">
         <v>60</v>
@@ -6071,7 +5964,7 @@
       <c r="AD27" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE27" s="81">
+      <c r="AE27" s="73">
         <v>1</v>
       </c>
       <c r="AF27" s="50">
@@ -6118,8 +6011,8 @@
       <c r="O28" s="50">
         <v>750</v>
       </c>
-      <c r="P28" s="78" t="s">
-        <v>514</v>
+      <c r="P28" s="70">
+        <v>0.4</v>
       </c>
       <c r="Q28" s="50">
         <v>40</v>
@@ -6163,7 +6056,7 @@
       <c r="AD28" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE28" s="81">
+      <c r="AE28" s="73">
         <v>9</v>
       </c>
       <c r="AF28" s="50">
@@ -6210,8 +6103,8 @@
       <c r="O29">
         <v>750</v>
       </c>
-      <c r="P29" s="78" t="s">
-        <v>515</v>
+      <c r="P29" s="70">
+        <v>0.42</v>
       </c>
       <c r="Q29">
         <v>60</v>
@@ -6255,7 +6148,7 @@
       <c r="AD29" s="50">
         <v>5</v>
       </c>
-      <c r="AE29" s="81">
+      <c r="AE29" s="73">
         <v>9</v>
       </c>
       <c r="AF29" s="50">
@@ -6302,8 +6195,8 @@
       <c r="O30">
         <v>700</v>
       </c>
-      <c r="P30" s="78" t="s">
-        <v>514</v>
+      <c r="P30" s="70">
+        <v>0.4</v>
       </c>
       <c r="Q30">
         <v>20</v>
@@ -6347,7 +6240,7 @@
       <c r="AD30" s="50">
         <v>5</v>
       </c>
-      <c r="AE30" s="81">
+      <c r="AE30" s="73">
         <v>9</v>
       </c>
       <c r="AF30" s="50">
@@ -6394,8 +6287,8 @@
       <c r="O31">
         <v>900</v>
       </c>
-      <c r="P31" s="78" t="s">
-        <v>514</v>
+      <c r="P31" s="70">
+        <v>0.4</v>
       </c>
       <c r="Q31">
         <v>60</v>
@@ -6439,7 +6332,7 @@
       <c r="AD31" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE31" s="81">
+      <c r="AE31" s="73">
         <v>9</v>
       </c>
       <c r="AF31" s="50">
@@ -6486,8 +6379,8 @@
       <c r="O32">
         <v>850</v>
       </c>
-      <c r="P32" s="78" t="s">
-        <v>501</v>
+      <c r="P32" s="70">
+        <v>0</v>
       </c>
       <c r="Q32">
         <v>60</v>
@@ -6531,7 +6424,7 @@
       <c r="AD32" s="50">
         <v>2.5</v>
       </c>
-      <c r="AE32" s="81">
+      <c r="AE32" s="73">
         <v>0</v>
       </c>
       <c r="AF32" s="50">
@@ -6578,8 +6471,8 @@
       <c r="O33">
         <v>950</v>
       </c>
-      <c r="P33" s="79" t="s">
-        <v>516</v>
+      <c r="P33" s="71">
+        <v>0.5</v>
       </c>
       <c r="Q33">
         <v>60</v>
@@ -6623,7 +6516,7 @@
       <c r="AD33" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE33" s="82">
+      <c r="AE33" s="74">
         <v>10</v>
       </c>
       <c r="AF33" s="50">
@@ -6670,8 +6563,8 @@
       <c r="O34">
         <v>800</v>
       </c>
-      <c r="P34" s="78" t="s">
-        <v>517</v>
+      <c r="P34" s="70">
+        <v>0.34300000000000003</v>
       </c>
       <c r="Q34">
         <v>60</v>
@@ -6715,7 +6608,7 @@
       <c r="AD34" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE34" s="81">
+      <c r="AE34" s="73">
         <v>3</v>
       </c>
       <c r="AF34" s="50">
@@ -6762,8 +6655,8 @@
       <c r="O35">
         <v>1200</v>
       </c>
-      <c r="P35" s="78" t="s">
-        <v>518</v>
+      <c r="P35" s="70">
+        <v>0.435</v>
       </c>
       <c r="Q35">
         <v>40</v>
@@ -6807,7 +6700,7 @@
       <c r="AD35" s="50">
         <v>10</v>
       </c>
-      <c r="AE35" s="81">
+      <c r="AE35" s="73">
         <v>9</v>
       </c>
       <c r="AF35" s="50">
@@ -6854,8 +6747,8 @@
       <c r="O36">
         <v>900</v>
       </c>
-      <c r="P36" s="78" t="s">
-        <v>519</v>
+      <c r="P36" s="70">
+        <v>0.48</v>
       </c>
       <c r="Q36">
         <v>40</v>
@@ -6899,7 +6792,7 @@
       <c r="AD36" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE36" s="81">
+      <c r="AE36" s="73">
         <v>10</v>
       </c>
       <c r="AF36" s="50">
@@ -6946,8 +6839,8 @@
       <c r="O37">
         <v>750</v>
       </c>
-      <c r="P37" s="78" t="s">
-        <v>520</v>
+      <c r="P37" s="70">
+        <v>0.44900000000000001</v>
       </c>
       <c r="Q37">
         <v>40</v>
@@ -6991,7 +6884,7 @@
       <c r="AD37" s="50">
         <v>10</v>
       </c>
-      <c r="AE37" s="81">
+      <c r="AE37" s="73">
         <v>9</v>
       </c>
       <c r="AF37" s="50">
@@ -7038,8 +6931,8 @@
       <c r="O38">
         <v>850</v>
       </c>
-      <c r="P38" s="79" t="s">
-        <v>521</v>
+      <c r="P38" s="71">
+        <v>0.53</v>
       </c>
       <c r="Q38">
         <v>60</v>
@@ -7083,7 +6976,7 @@
       <c r="AD38" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE38" s="82">
+      <c r="AE38" s="74">
         <v>10</v>
       </c>
       <c r="AF38" s="50">
@@ -7130,8 +7023,8 @@
       <c r="O39">
         <v>800</v>
       </c>
-      <c r="P39" s="78" t="s">
-        <v>522</v>
+      <c r="P39" s="70">
+        <v>0.44400000000000001</v>
       </c>
       <c r="Q39">
         <v>60</v>
@@ -7175,7 +7068,7 @@
       <c r="AD39" s="50">
         <v>3.75</v>
       </c>
-      <c r="AE39" s="81">
+      <c r="AE39" s="73">
         <v>9</v>
       </c>
       <c r="AF39" s="50">
@@ -7222,8 +7115,8 @@
       <c r="O40">
         <v>750</v>
       </c>
-      <c r="P40" s="80" t="s">
-        <v>523</v>
+      <c r="P40" s="72">
+        <v>0.88600000000000001</v>
       </c>
       <c r="Q40">
         <v>60</v>
@@ -7267,7 +7160,7 @@
       <c r="AD40" s="50">
         <v>7</v>
       </c>
-      <c r="AE40" s="83">
+      <c r="AE40" s="75">
         <v>10</v>
       </c>
       <c r="AF40" s="50">
@@ -7314,8 +7207,8 @@
       <c r="O41">
         <v>750</v>
       </c>
-      <c r="P41" s="78" t="s">
-        <v>524</v>
+      <c r="P41" s="70">
+        <v>0.41299999999999998</v>
       </c>
       <c r="Q41">
         <v>80</v>
@@ -7359,7 +7252,7 @@
       <c r="AD41" s="50">
         <v>5</v>
       </c>
-      <c r="AE41" s="81">
+      <c r="AE41" s="73">
         <v>9</v>
       </c>
       <c r="AF41" s="50">
@@ -7406,8 +7299,8 @@
       <c r="O42">
         <v>750</v>
       </c>
-      <c r="P42" s="78" t="s">
-        <v>515</v>
+      <c r="P42" s="70">
+        <v>0.42</v>
       </c>
       <c r="Q42">
         <v>40</v>
@@ -7451,7 +7344,7 @@
       <c r="AD42" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE42" s="81">
+      <c r="AE42" s="73">
         <v>9</v>
       </c>
       <c r="AF42" s="50">
@@ -7498,8 +7391,8 @@
       <c r="O43">
         <v>700</v>
       </c>
-      <c r="P43" s="78" t="s">
-        <v>525</v>
+      <c r="P43" s="70">
+        <v>0.42399999999999999</v>
       </c>
       <c r="Q43">
         <v>20</v>
@@ -7543,7 +7436,7 @@
       <c r="AD43" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE43" s="81">
+      <c r="AE43" s="73">
         <v>9</v>
       </c>
       <c r="AF43" s="50">
@@ -7590,8 +7483,8 @@
       <c r="O44">
         <v>850</v>
       </c>
-      <c r="P44" s="78" t="s">
-        <v>526</v>
+      <c r="P44" s="70">
+        <v>0.40500000000000003</v>
       </c>
       <c r="Q44">
         <v>20</v>
@@ -7635,7 +7528,7 @@
       <c r="AD44" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE44" s="81">
+      <c r="AE44" s="73">
         <v>9</v>
       </c>
       <c r="AF44" s="50">
@@ -7682,8 +7575,8 @@
       <c r="O45">
         <v>650</v>
       </c>
-      <c r="P45" s="78" t="s">
-        <v>527</v>
+      <c r="P45" s="70">
+        <v>0.47399999999999998</v>
       </c>
       <c r="Q45">
         <v>80</v>
@@ -7727,7 +7620,7 @@
       <c r="AD45" s="50">
         <v>10</v>
       </c>
-      <c r="AE45" s="81">
+      <c r="AE45" s="73">
         <v>10</v>
       </c>
       <c r="AF45" s="50">
@@ -7774,8 +7667,8 @@
       <c r="O46">
         <v>510</v>
       </c>
-      <c r="P46" s="78" t="s">
-        <v>508</v>
+      <c r="P46" s="70">
+        <v>0.35</v>
       </c>
       <c r="Q46">
         <v>60</v>
@@ -7819,7 +7712,7 @@
       <c r="AD46" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE46" s="81">
+      <c r="AE46" s="73">
         <v>3</v>
       </c>
       <c r="AF46" s="50">
@@ -7866,8 +7759,8 @@
       <c r="O47">
         <v>510</v>
       </c>
-      <c r="P47" s="78" t="s">
-        <v>504</v>
+      <c r="P47" s="70">
+        <v>0.33300000000000002</v>
       </c>
       <c r="Q47">
         <v>60</v>
@@ -7911,7 +7804,7 @@
       <c r="AD47" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE47" s="81">
+      <c r="AE47" s="73">
         <v>1</v>
       </c>
       <c r="AF47" s="50">
@@ -7958,8 +7851,8 @@
       <c r="O48">
         <v>350</v>
       </c>
-      <c r="P48" s="78" t="s">
-        <v>504</v>
+      <c r="P48" s="70">
+        <v>0.33300000000000002</v>
       </c>
       <c r="Q48">
         <v>40</v>
@@ -8003,7 +7896,7 @@
       <c r="AD48" s="50">
         <v>5</v>
       </c>
-      <c r="AE48" s="81">
+      <c r="AE48" s="73">
         <v>1</v>
       </c>
       <c r="AF48" s="50">
@@ -8050,8 +7943,8 @@
       <c r="O49">
         <v>535</v>
       </c>
-      <c r="P49" s="78" t="s">
-        <v>528</v>
+      <c r="P49" s="70">
+        <v>0.42899999999999999</v>
       </c>
       <c r="Q49">
         <v>30</v>
@@ -8095,7 +7988,7 @@
       <c r="AD49" s="50">
         <v>3.75</v>
       </c>
-      <c r="AE49" s="81">
+      <c r="AE49" s="73">
         <v>9</v>
       </c>
       <c r="AF49" s="50">
@@ -8142,8 +8035,8 @@
       <c r="O50">
         <v>530</v>
       </c>
-      <c r="P50" s="78" t="s">
-        <v>529</v>
+      <c r="P50" s="70">
+        <v>0.41699999999999998</v>
       </c>
       <c r="Q50">
         <v>60</v>
@@ -8187,7 +8080,7 @@
       <c r="AD50" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE50" s="81">
+      <c r="AE50" s="73">
         <v>9</v>
       </c>
       <c r="AF50" s="50">
@@ -8234,8 +8127,8 @@
       <c r="O51">
         <v>485</v>
       </c>
-      <c r="P51" s="78" t="s">
-        <v>530</v>
+      <c r="P51" s="70">
+        <v>0.35699999999999998</v>
       </c>
       <c r="Q51">
         <v>60</v>
@@ -8279,7 +8172,7 @@
       <c r="AD51" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE51" s="81">
+      <c r="AE51" s="73">
         <v>5</v>
       </c>
       <c r="AF51" s="50">
@@ -8326,8 +8219,8 @@
       <c r="O52">
         <v>550</v>
       </c>
-      <c r="P52" s="78" t="s">
-        <v>531</v>
+      <c r="P52" s="70">
+        <v>0.39300000000000002</v>
       </c>
       <c r="Q52">
         <v>28</v>
@@ -8371,7 +8264,7 @@
       <c r="AD52" s="50">
         <v>3.5</v>
       </c>
-      <c r="AE52" s="81">
+      <c r="AE52" s="73">
         <v>9</v>
       </c>
       <c r="AF52" s="50">
@@ -8418,8 +8311,8 @@
       <c r="O53">
         <v>675</v>
       </c>
-      <c r="P53" s="78" t="s">
-        <v>524</v>
+      <c r="P53" s="70">
+        <v>0.41299999999999998</v>
       </c>
       <c r="Q53" t="s">
         <v>266</v>
@@ -8463,7 +8356,7 @@
       <c r="AD53" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE53" s="81">
+      <c r="AE53" s="73">
         <v>9</v>
       </c>
       <c r="AF53" s="50">
@@ -8507,8 +8400,8 @@
       <c r="O54">
         <v>750</v>
       </c>
-      <c r="P54" s="79" t="s">
-        <v>516</v>
+      <c r="P54" s="71">
+        <v>0.5</v>
       </c>
       <c r="Q54" t="s">
         <v>274</v>
@@ -8552,7 +8445,7 @@
       <c r="AD54" s="50">
         <v>5</v>
       </c>
-      <c r="AE54" s="82">
+      <c r="AE54" s="74">
         <v>10</v>
       </c>
       <c r="AF54" s="50">
@@ -8599,8 +8492,8 @@
       <c r="O55">
         <v>800</v>
       </c>
-      <c r="P55" s="78" t="s">
-        <v>508</v>
+      <c r="P55" s="70">
+        <v>0.35</v>
       </c>
       <c r="Q55">
         <v>60</v>
@@ -8644,7 +8537,7 @@
       <c r="AD55" s="50">
         <v>5</v>
       </c>
-      <c r="AE55" s="81">
+      <c r="AE55" s="73">
         <v>3</v>
       </c>
       <c r="AF55" s="50">
@@ -8691,8 +8584,8 @@
       <c r="O56">
         <v>700</v>
       </c>
-      <c r="P56" s="79" t="s">
-        <v>516</v>
+      <c r="P56" s="71">
+        <v>0.5</v>
       </c>
       <c r="Q56">
         <v>56</v>
@@ -8736,7 +8629,7 @@
       <c r="AD56" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE56" s="82">
+      <c r="AE56" s="74">
         <v>10</v>
       </c>
       <c r="AF56" s="50">
@@ -8783,8 +8676,8 @@
       <c r="O57">
         <v>625</v>
       </c>
-      <c r="P57" s="78" t="s">
-        <v>514</v>
+      <c r="P57" s="70">
+        <v>0.4</v>
       </c>
       <c r="Q57">
         <v>60</v>
@@ -8828,7 +8721,7 @@
       <c r="AD57" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE57" s="81">
+      <c r="AE57" s="73">
         <v>9</v>
       </c>
       <c r="AF57" s="50">
@@ -8872,8 +8765,8 @@
       <c r="O58">
         <v>650</v>
       </c>
-      <c r="P58" s="78" t="s">
-        <v>529</v>
+      <c r="P58" s="70">
+        <v>0.41699999999999998</v>
       </c>
       <c r="R58" s="50">
         <v>3</v>
@@ -8914,7 +8807,7 @@
       <c r="AD58" s="50">
         <v>4</v>
       </c>
-      <c r="AE58" s="81">
+      <c r="AE58" s="73">
         <v>9</v>
       </c>
       <c r="AF58" s="50">
@@ -8961,8 +8854,8 @@
       <c r="O59">
         <v>704</v>
       </c>
-      <c r="P59" s="78" t="s">
-        <v>501</v>
+      <c r="P59" s="70">
+        <v>0</v>
       </c>
       <c r="Q59">
         <v>80</v>
@@ -9006,7 +8899,7 @@
       <c r="AD59" s="50">
         <v>0.625</v>
       </c>
-      <c r="AE59" s="81">
+      <c r="AE59" s="73">
         <v>0</v>
       </c>
       <c r="AF59" s="50">
@@ -9053,8 +8946,8 @@
       <c r="O60">
         <v>704</v>
       </c>
-      <c r="P60" s="78" t="s">
-        <v>501</v>
+      <c r="P60" s="70">
+        <v>0</v>
       </c>
       <c r="Q60">
         <v>30</v>
@@ -9098,7 +8991,7 @@
       <c r="AD60" s="50">
         <v>5</v>
       </c>
-      <c r="AE60" s="81">
+      <c r="AE60" s="73">
         <v>0</v>
       </c>
       <c r="AF60" s="50">
@@ -9145,8 +9038,8 @@
       <c r="O61">
         <v>700</v>
       </c>
-      <c r="P61" s="78" t="s">
-        <v>514</v>
+      <c r="P61" s="70">
+        <v>0.4</v>
       </c>
       <c r="Q61">
         <v>60</v>
@@ -9190,7 +9083,7 @@
       <c r="AD61" s="50">
         <v>7.5</v>
       </c>
-      <c r="AE61" s="81">
+      <c r="AE61" s="73">
         <v>9</v>
       </c>
       <c r="AF61" s="50">
@@ -9237,8 +9130,8 @@
       <c r="O62">
         <v>650</v>
       </c>
-      <c r="P62" s="78" t="s">
-        <v>532</v>
+      <c r="P62" s="70">
+        <v>0.438</v>
       </c>
       <c r="Q62" t="s">
         <v>321</v>
@@ -9282,7 +9175,7 @@
       <c r="AD62" s="50">
         <v>2.5</v>
       </c>
-      <c r="AE62" s="81">
+      <c r="AE62" s="73">
         <v>9</v>
       </c>
       <c r="AF62" s="50">
@@ -9329,8 +9222,8 @@
       <c r="O63">
         <v>670</v>
       </c>
-      <c r="P63" s="78" t="s">
-        <v>514</v>
+      <c r="P63" s="70">
+        <v>0.4</v>
       </c>
       <c r="Q63" t="s">
         <v>327</v>
@@ -9374,7 +9267,7 @@
       <c r="AD63" s="50">
         <v>1.5</v>
       </c>
-      <c r="AE63" s="81">
+      <c r="AE63" s="73">
         <v>9</v>
       </c>
       <c r="AF63" s="50">
@@ -9421,8 +9314,8 @@
       <c r="O64">
         <v>700</v>
       </c>
-      <c r="P64" s="78" t="s">
-        <v>501</v>
+      <c r="P64" s="70">
+        <v>0</v>
       </c>
       <c r="Q64">
         <v>60</v>
@@ -9466,7 +9359,7 @@
       <c r="AD64" s="50">
         <v>2.5</v>
       </c>
-      <c r="AE64" s="81">
+      <c r="AE64" s="73">
         <v>0</v>
       </c>
       <c r="AF64" s="50">
@@ -9513,8 +9406,8 @@
       <c r="O65">
         <v>795</v>
       </c>
-      <c r="P65" s="78" t="s">
-        <v>533</v>
+      <c r="P65" s="70">
+        <v>0.25</v>
       </c>
       <c r="Q65">
         <v>60</v>
@@ -9558,7 +9451,7 @@
       <c r="AD65" s="50">
         <v>2.5</v>
       </c>
-      <c r="AE65" s="81">
+      <c r="AE65" s="73">
         <v>1</v>
       </c>
       <c r="AF65" s="50">
@@ -9602,30 +9495,30 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>339</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="69"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9646,30 +9539,30 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>340</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="69"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9690,30 +9583,30 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>341</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="69"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9764,17 +9657,17 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="78" t="s">
         <v>346</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="78" t="s">
         <v>347</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="78" t="s">
         <v>348</v>
       </c>
-      <c r="E2" s="70" t="s">
+      <c r="E2" s="78" t="s">
         <v>349</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -9782,11 +9675,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="70"/>
+      <c r="A3" s="78"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
       <c r="F3" s="2" t="s">
         <v>351</v>
       </c>
@@ -9922,17 +9815,17 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="78" t="s">
         <v>379</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="70" t="s">
+      <c r="C11" s="78" t="s">
         <v>380</v>
       </c>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="78" t="s">
         <v>381</v>
       </c>
-      <c r="E11" s="70" t="s">
+      <c r="E11" s="78" t="s">
         <v>382</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -9940,11 +9833,11 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="70"/>
+      <c r="A12" s="78"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
       <c r="F12" s="2" t="s">
         <v>384</v>
       </c>
@@ -9986,30 +9879,30 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="78" t="s">
         <v>395</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="70" t="s">
+      <c r="C15" s="78" t="s">
         <v>396</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="D15" s="78" t="s">
         <v>397</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="E15" s="78" t="s">
         <v>398</v>
       </c>
-      <c r="F15" s="70" t="s">
+      <c r="F15" s="78" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="70"/>
+      <c r="A16" s="78"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
@@ -10030,7 +9923,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="71" t="s">
+      <c r="A18" s="79" t="s">
         <v>405</v>
       </c>
       <c r="B18" s="24"/>
@@ -10051,7 +9944,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="71"/>
+      <c r="A19" s="79"/>
       <c r="B19" s="24"/>
       <c r="C19" s="18" t="s">
         <v>411</v>
@@ -10067,7 +9960,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="71"/>
+      <c r="A20" s="79"/>
       <c r="B20" s="24"/>
       <c r="C20" s="18" t="s">
         <v>415</v>
@@ -10083,7 +9976,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="71"/>
+      <c r="A21" s="79"/>
       <c r="B21" s="24"/>
       <c r="C21" s="18" t="s">
         <v>417</v>

</xml_diff>